<commit_message>
Support for any other fields
</commit_message>
<xml_diff>
--- a/excel-test-source-plugin/SampleProject/ExcelTestSource1.xlsx
+++ b/excel-test-source-plugin/SampleProject/ExcelTestSource1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\SpecSync\Samples\specsync-sample-plugins\excel-test-source-plugin\SampleProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626B565A-E2DF-4574-B624-59FF13FBA1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B50E7F-DD09-4B95-9AB8-1FB18231DAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -132,6 +132,18 @@
   </si>
   <si>
     <t>Other Script</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>specsync-plugins-demo\Area2\Area 2.1</t>
+  </si>
+  <si>
+    <t>tag1</t>
+  </si>
+  <si>
+    <t>Ready</t>
   </si>
 </sst>
 </file>
@@ -615,12 +627,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -666,7 +677,12 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -741,22 +757,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:M12" totalsRowShown="0">
-  <autoFilter ref="A1:M12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Work Item Type" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Title" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Test Step" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Step Action" dataDxfId="7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:N12" totalsRowShown="0">
+  <autoFilter ref="A1:N12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Work Item Type" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Title" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Test Step" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Step Action" dataDxfId="8"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Step Expected"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Area Path" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Assigned To" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="State" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Tags" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{9100DF04-DA71-4007-AAD8-F31E557CE8F1}" name="Description" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{0F1EA86D-F0D9-4C17-9E92-41FB9D95D737}" name="Automation Status" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{1297D201-E5D5-4738-A4EE-10ECBF7BBBCB}" name="Automated Test Name" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Area Path" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Assigned To" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="State" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Tags" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{9100DF04-DA71-4007-AAD8-F31E557CE8F1}" name="Description" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{0F1EA86D-F0D9-4C17-9E92-41FB9D95D737}" name="Automation Status" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{1297D201-E5D5-4738-A4EE-10ECBF7BBBCB}" name="Automated Test Name" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{26F7B37D-7A7E-41CD-9AE1-A759FAC91BBB}" name="Priority" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1059,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,7 +1098,7 @@
     <col min="13" max="13" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1121,8 +1138,11 @@
       <c r="M1" t="s">
         <v>34</v>
       </c>
+      <c r="N1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>124</v>
       </c>
@@ -1133,7 +1153,7 @@
         <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -1147,12 +1167,14 @@
       <c r="K2" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="2"/>
+      <c r="N2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>1</v>
       </c>
@@ -1162,10 +1184,8 @@
       <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>2</v>
       </c>
@@ -1175,10 +1195,8 @@
       <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>3</v>
       </c>
@@ -1188,10 +1206,8 @@
       <c r="F5" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>125</v>
       </c>
@@ -1211,16 +1227,19 @@
         <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" t="s">
         <v>35</v>
       </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>1</v>
       </c>
@@ -1230,10 +1249,8 @@
       <c r="F7" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>2</v>
       </c>
@@ -1243,10 +1260,8 @@
       <c r="F8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>3</v>
       </c>
@@ -1256,27 +1271,34 @@
       <c r="F9" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>130</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
       </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" t="s">
+        <v>40</v>
+      </c>
       <c r="J10" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" t="s">
         <v>33</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="M10" t="s">
         <v>36</v>
       </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>1</v>
       </c>
@@ -1286,10 +1308,8 @@
       <c r="F11" t="s">
         <v>25</v>
       </c>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>2</v>
       </c>
@@ -1299,8 +1319,6 @@
       <c r="F12" t="s">
         <v>27</v>
       </c>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ExcelTestSource plugin: allow defining first step in test case row, improve flexibility (#1342)
</commit_message>
<xml_diff>
--- a/excel-test-source-plugin/SampleProject/ExcelTestSource1.xlsx
+++ b/excel-test-source-plugin/SampleProject/ExcelTestSource1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\SpecSync\Samples\specsync-sample-plugins\excel-test-source-plugin\SampleProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\SpecSync\SpecSync\Plugins\excel-test-source-plugin\SampleProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746F3CDA-C2AD-4AB2-8402-F2878838D1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF00DC51-12BA-4624-8B17-F7FD6D204087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExcelTestSource_ExcelTestSource" sheetId="1" r:id="rId1"/>
@@ -757,8 +757,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:N12" totalsRowShown="0">
-  <autoFilter ref="A1:N12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:N11" totalsRowShown="0">
+  <autoFilter ref="A1:N11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Work Item Type" dataDxfId="11"/>
@@ -1076,17 +1076,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="33.140625" customWidth="1"/>
@@ -1279,6 +1279,15 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
       <c r="G10" t="s">
         <v>12</v>
       </c>
@@ -1300,23 +1309,12 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update version of SpecSync.Plugin.ExcelTestSource to v1.1.0
</commit_message>
<xml_diff>
--- a/excel-test-source-plugin/SampleProject/ExcelTestSource1.xlsx
+++ b/excel-test-source-plugin/SampleProject/ExcelTestSource1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\SpecSync\SpecSync\Plugins\excel-test-source-plugin\SampleProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF00DC51-12BA-4624-8B17-F7FD6D204087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9602969E-F46D-4F78-8B89-631AB6B80EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExcelTestSource_ExcelTestSource" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -92,24 +92,6 @@
     <t>Test Case 2</t>
   </si>
   <si>
-    <t>New Test Case from Excel again</t>
-  </si>
-  <si>
-    <t>Do this</t>
-  </si>
-  <si>
-    <t>Verify that</t>
-  </si>
-  <si>
-    <t>Do this as well</t>
-  </si>
-  <si>
-    <t>Verify that as well</t>
-  </si>
-  <si>
-    <t>otherTag, story:131</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -128,9 +110,6 @@
     <t>Stript 1</t>
   </si>
   <si>
-    <t>Other Script</t>
-  </si>
-  <si>
     <t>Priority</t>
   </si>
   <si>
@@ -138,9 +117,6 @@
   </si>
   <si>
     <t>tag1</t>
-  </si>
-  <si>
-    <t>Ready</t>
   </si>
   <si>
     <t>Not Automated</t>
@@ -757,8 +733,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:N11" totalsRowShown="0">
-  <autoFilter ref="A1:N11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:N9" totalsRowShown="0">
+  <autoFilter ref="A1:N9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Work Item Type" dataDxfId="11"/>
@@ -1076,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,16 +1106,16 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
         <v>29</v>
-      </c>
-      <c r="L1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1153,7 +1129,7 @@
         <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -1165,10 +1141,10 @@
         <v>15</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="L2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="N2">
         <v>2</v>
@@ -1227,13 +1203,13 @@
         <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="L6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="M6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="N6">
         <v>3</v>
@@ -1270,52 +1246,6 @@
       </c>
       <c r="F9" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>130</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" t="s">
-        <v>28</v>
-      </c>
-      <c r="L10" t="s">
-        <v>32</v>
-      </c>
-      <c r="M10" t="s">
-        <v>35</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>